<commit_message>
Update with new logics
</commit_message>
<xml_diff>
--- a/consolidated_forecast_WITH_PO.xlsx
+++ b/consolidated_forecast_WITH_PO.xlsx
@@ -7,8 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="No ASIN" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08F7BHDLY" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="No ASIN" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -417,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -428,537 +429,693 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>product title</t>
+          <t>Week</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>week</t>
+          <t>Week_Start_Date</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>year</t>
+          <t>ASIN</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>y</t>
+          <t>MyForecast</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>asin</t>
+          <t>Amazon Mean Forecast</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>ds</t>
+          <t>Amazon P70 Forecast</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Amazon P80 Forecast</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Amazon P90 Forecast</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Product Title</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>is_holiday_week</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>GS27QC SA</t>
+          <t>W1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>W06</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>2023</v>
+          <t>2025-02-02</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>B08F7BHDLY</t>
+        </is>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>105</v>
       </c>
       <c r="E2" t="n">
-        <v/>
-      </c>
-      <c r="F2" s="1" t="n">
-        <v>44955</v>
+        <v>81</v>
+      </c>
+      <c r="F2" t="n">
+        <v>92</v>
+      </c>
+      <c r="G2" t="n">
+        <v>102</v>
+      </c>
+      <c r="H2" t="n">
+        <v>116</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>A520I AC</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>GS27F SA</t>
+          <t>W2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>W07</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>2023</v>
+          <t>2025-02-09</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>B08F7BHDLY</t>
+        </is>
       </c>
       <c r="D3" t="n">
-        <v>36</v>
+        <v>100</v>
       </c>
       <c r="E3" t="n">
-        <v/>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>44962</v>
+        <v>82</v>
+      </c>
+      <c r="F3" t="n">
+        <v>95</v>
+      </c>
+      <c r="G3" t="n">
+        <v>105</v>
+      </c>
+      <c r="H3" t="n">
+        <v>121</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>A520I AC</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v/>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>GS27FC SA</t>
+          <t>W3</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>W07</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>2023</v>
+          <t>2025-02-16</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>B08F7BHDLY</t>
+        </is>
       </c>
       <c r="D4" t="n">
-        <v>5</v>
+        <v>96</v>
       </c>
       <c r="E4" t="n">
-        <v/>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>44962</v>
+        <v>86</v>
+      </c>
+      <c r="F4" t="n">
+        <v>100</v>
+      </c>
+      <c r="G4" t="n">
+        <v>111</v>
+      </c>
+      <c r="H4" t="n">
+        <v>128</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>A520I AC</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v/>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>GS27F SA</t>
+          <t>W4</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>W07</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>2023</v>
+          <t>2025-02-23</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>B08F7BHDLY</t>
+        </is>
       </c>
       <c r="D5" t="n">
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="E5" t="n">
-        <v/>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>44962</v>
+        <v>87</v>
+      </c>
+      <c r="F5" t="n">
+        <v>101</v>
+      </c>
+      <c r="G5" t="n">
+        <v>113</v>
+      </c>
+      <c r="H5" t="n">
+        <v>132</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>A520I AC</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v/>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">GS27QC SA                     </t>
+          <t>W5</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>W32</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>2023</v>
+          <t>2025-03-02</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>B08F7BHDLY</t>
+        </is>
       </c>
       <c r="D6" t="n">
-        <v>4</v>
+        <v>113</v>
       </c>
       <c r="E6" t="n">
-        <v/>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>45137</v>
+        <v>87</v>
+      </c>
+      <c r="F6" t="n">
+        <v>102</v>
+      </c>
+      <c r="G6" t="n">
+        <v>116</v>
+      </c>
+      <c r="H6" t="n">
+        <v>137</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>A520I AC</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v/>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve">GS27QC SA                     </t>
+          <t>W6</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>W33</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>2023</v>
+          <t>2025-03-09</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>B08F7BHDLY</t>
+        </is>
       </c>
       <c r="D7" t="n">
-        <v>15</v>
+        <v>112</v>
       </c>
       <c r="E7" t="n">
-        <v/>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>45144</v>
+        <v>86</v>
+      </c>
+      <c r="F7" t="n">
+        <v>101</v>
+      </c>
+      <c r="G7" t="n">
+        <v>114</v>
+      </c>
+      <c r="H7" t="n">
+        <v>135</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>A520I AC</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v/>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve">GS27QC SA                     </t>
+          <t>W7</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>W34</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>2023</v>
+          <t>2025-03-16</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>B08F7BHDLY</t>
+        </is>
       </c>
       <c r="D8" t="n">
-        <v>14</v>
+        <v>109</v>
       </c>
       <c r="E8" t="n">
-        <v/>
-      </c>
-      <c r="F8" s="1" t="n">
-        <v>45151</v>
+        <v>84</v>
+      </c>
+      <c r="F8" t="n">
+        <v>99</v>
+      </c>
+      <c r="G8" t="n">
+        <v>114</v>
+      </c>
+      <c r="H8" t="n">
+        <v>137</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>A520I AC</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v/>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve">GS27QC SA                     </t>
+          <t>W8</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>W35</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>2023</v>
+          <t>2025-03-23</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>B08F7BHDLY</t>
+        </is>
       </c>
       <c r="D9" t="n">
-        <v>23</v>
+        <v>95</v>
       </c>
       <c r="E9" t="n">
-        <v/>
-      </c>
-      <c r="F9" s="1" t="n">
-        <v>45158</v>
+        <v>85</v>
+      </c>
+      <c r="F9" t="n">
+        <v>102</v>
+      </c>
+      <c r="G9" t="n">
+        <v>118</v>
+      </c>
+      <c r="H9" t="n">
+        <v>142</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>A520I AC</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v/>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve">GS27QC SA                     </t>
+          <t>W9</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>W36</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>2023</v>
+          <t>2025-03-30</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>B08F7BHDLY</t>
+        </is>
       </c>
       <c r="D10" t="n">
-        <v>4</v>
+        <v>86</v>
       </c>
       <c r="E10" t="n">
-        <v/>
-      </c>
-      <c r="F10" s="1" t="n">
-        <v>45165</v>
+        <v>84</v>
+      </c>
+      <c r="F10" t="n">
+        <v>100</v>
+      </c>
+      <c r="G10" t="n">
+        <v>115</v>
+      </c>
+      <c r="H10" t="n">
+        <v>137</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>A520I AC</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v/>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve">GS27F SA                      </t>
+          <t>W10</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>W37</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>2023</v>
+          <t>2025-04-06</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>B08F7BHDLY</t>
+        </is>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>94</v>
       </c>
       <c r="E11" t="n">
-        <v/>
-      </c>
-      <c r="F11" s="1" t="n">
-        <v>45172</v>
+        <v>80</v>
+      </c>
+      <c r="F11" t="n">
+        <v>96</v>
+      </c>
+      <c r="G11" t="n">
+        <v>112</v>
+      </c>
+      <c r="H11" t="n">
+        <v>137</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>A520I AC</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v/>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve">GS27FC SA </t>
+          <t>W11</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>W37</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>2023</v>
+          <t>2025-04-13</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>B08F7BHDLY</t>
+        </is>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="E12" t="n">
-        <v/>
-      </c>
-      <c r="F12" s="1" t="n">
-        <v>45172</v>
+        <v>81</v>
+      </c>
+      <c r="F12" t="n">
+        <v>97</v>
+      </c>
+      <c r="G12" t="n">
+        <v>114</v>
+      </c>
+      <c r="H12" t="n">
+        <v>139</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>A520I AC</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v/>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve">GS27QC SA                     </t>
+          <t>W12</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>W37</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>2023</v>
+          <t>2025-04-20</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>B08F7BHDLY</t>
+        </is>
       </c>
       <c r="D13" t="n">
-        <v>2</v>
+        <v>105</v>
       </c>
       <c r="E13" t="n">
-        <v/>
-      </c>
-      <c r="F13" s="1" t="n">
-        <v>45172</v>
+        <v>81</v>
+      </c>
+      <c r="F13" t="n">
+        <v>97</v>
+      </c>
+      <c r="G13" t="n">
+        <v>114</v>
+      </c>
+      <c r="H13" t="n">
+        <v>139</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>A520I AC</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v/>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t xml:space="preserve">GS27F SA                      </t>
+          <t>W13</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>W38</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>2023</v>
+          <t>2025-04-27</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>B08F7BHDLY</t>
+        </is>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>103</v>
       </c>
       <c r="E14" t="n">
-        <v/>
-      </c>
-      <c r="F14" s="1" t="n">
-        <v>45179</v>
+        <v>80</v>
+      </c>
+      <c r="F14" t="n">
+        <v>95</v>
+      </c>
+      <c r="G14" t="n">
+        <v>111</v>
+      </c>
+      <c r="H14" t="n">
+        <v>136</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>A520I AC</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v/>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t xml:space="preserve">GS27FC SA                     </t>
+          <t>W14</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>W38</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>2023</v>
+          <t>2025-05-04</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>B08F7BHDLY</t>
+        </is>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E15" t="n">
-        <v/>
-      </c>
-      <c r="F15" s="1" t="n">
-        <v>45179</v>
+        <v>75</v>
+      </c>
+      <c r="F15" t="n">
+        <v>90</v>
+      </c>
+      <c r="G15" t="n">
+        <v>106</v>
+      </c>
+      <c r="H15" t="n">
+        <v>132</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>A520I AC</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v/>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t xml:space="preserve">GS27QC SA                     </t>
+          <t>W15</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>W38</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>2023</v>
+          <t>2025-05-11</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>B08F7BHDLY</t>
+        </is>
       </c>
       <c r="D16" t="n">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="E16" t="n">
-        <v/>
-      </c>
-      <c r="F16" s="1" t="n">
-        <v>45179</v>
+        <v>75</v>
+      </c>
+      <c r="F16" t="n">
+        <v>90</v>
+      </c>
+      <c r="G16" t="n">
+        <v>105</v>
+      </c>
+      <c r="H16" t="n">
+        <v>129</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>A520I AC</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v/>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve">GS27F SA                      </t>
+          <t>W16</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>W39</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>2023</v>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>B08F7BHDLY</t>
+        </is>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="E17" t="n">
-        <v/>
-      </c>
-      <c r="F17" s="1" t="n">
-        <v>45186</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t xml:space="preserve">GS27FC SA                     </t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>W39</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>2023</v>
-      </c>
-      <c r="D18" t="n">
-        <v>2</v>
-      </c>
-      <c r="E18" t="n">
-        <v/>
-      </c>
-      <c r="F18" s="1" t="n">
-        <v>45186</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">GS27QC SA                     </t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>W39</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>2023</v>
-      </c>
-      <c r="D19" t="n">
-        <v>25</v>
-      </c>
-      <c r="E19" t="n">
-        <v/>
-      </c>
-      <c r="F19" s="1" t="n">
-        <v>45186</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t xml:space="preserve">GS27F SA                      </t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>W40</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>2023</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" t="n">
-        <v/>
-      </c>
-      <c r="F20" s="1" t="n">
-        <v>45193</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t xml:space="preserve">GS27FC SA                     </t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>W40</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>2023</v>
-      </c>
-      <c r="D21" t="n">
-        <v>1</v>
-      </c>
-      <c r="E21" t="n">
-        <v/>
-      </c>
-      <c r="F21" s="1" t="n">
-        <v>45193</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t xml:space="preserve">GS27QC SA                     </t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>W40</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>2023</v>
-      </c>
-      <c r="D22" t="n">
-        <v>71</v>
-      </c>
-      <c r="E22" t="n">
-        <v/>
-      </c>
-      <c r="F22" s="1" t="n">
-        <v>45193</v>
+        <v>74</v>
+      </c>
+      <c r="F17" t="n">
+        <v>89</v>
+      </c>
+      <c r="G17" t="n">
+        <v>105</v>
+      </c>
+      <c r="H17" t="n">
+        <v>130</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>A520I AC</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -972,7 +1129,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -983,6 +1140,561 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>product title</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>week</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>asin</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>ds</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>GS27QC SA</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>W06</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" t="n">
+        <v/>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>44955</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>GS27F SA</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>W07</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D3" t="n">
+        <v>36</v>
+      </c>
+      <c r="E3" t="n">
+        <v/>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>44962</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>GS27FC SA</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>W07</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D4" t="n">
+        <v>5</v>
+      </c>
+      <c r="E4" t="n">
+        <v/>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>44962</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>GS27F SA</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>W07</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D5" t="n">
+        <v>9</v>
+      </c>
+      <c r="E5" t="n">
+        <v/>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>44962</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GS27QC SA                     </t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>W32</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" t="n">
+        <v/>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>45137</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GS27QC SA                     </t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>W33</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D7" t="n">
+        <v>15</v>
+      </c>
+      <c r="E7" t="n">
+        <v/>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>45144</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GS27QC SA                     </t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>W34</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D8" t="n">
+        <v>14</v>
+      </c>
+      <c r="E8" t="n">
+        <v/>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>45151</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GS27QC SA                     </t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>W35</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D9" t="n">
+        <v>23</v>
+      </c>
+      <c r="E9" t="n">
+        <v/>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>45158</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GS27QC SA                     </t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>W36</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D10" t="n">
+        <v>4</v>
+      </c>
+      <c r="E10" t="n">
+        <v/>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>45165</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GS27F SA                      </t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>W37</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v/>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>45172</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GS27FC SA </t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>W37</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v/>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>45172</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GS27QC SA                     </t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>W37</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" t="n">
+        <v/>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>45172</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GS27F SA                      </t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>W38</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v/>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>45179</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GS27FC SA                     </t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>W38</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v/>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>45179</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GS27QC SA                     </t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>W38</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D16" t="n">
+        <v>11</v>
+      </c>
+      <c r="E16" t="n">
+        <v/>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>45179</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GS27F SA                      </t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>W39</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v/>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>45186</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GS27FC SA                     </t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>W39</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2</v>
+      </c>
+      <c r="E18" t="n">
+        <v/>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>45186</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GS27QC SA                     </t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>W39</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D19" t="n">
+        <v>25</v>
+      </c>
+      <c r="E19" t="n">
+        <v/>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>45186</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GS27F SA                      </t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>W40</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v/>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>45193</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GS27FC SA                     </t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>W40</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" t="n">
+        <v/>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>45193</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GS27QC SA                     </t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>W40</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D22" t="n">
+        <v>71</v>
+      </c>
+      <c r="E22" t="n">
+        <v/>
+      </c>
+      <c r="F22" s="1" t="n">
+        <v>45193</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>ASIN</t>
         </is>
       </c>
@@ -1005,6 +1717,27 @@
         <is>
           <t>16 Week Forecast</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>B08F7BHDLY</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>A520I AC</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>407.3</v>
+      </c>
+      <c r="D2" t="n">
+        <v>836.4000000000001</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1588</v>
       </c>
     </row>
   </sheetData>

</xml_diff>